<commit_message>
Fixed quaterly metric growth calculations to look back to the same quarter in the previous FY
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/AAPL/quarter/stock_price_data.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/AAPL/quarter/stock_price_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>high</t>
   </si>
@@ -26,63 +26,6 @@
   </si>
   <si>
     <t>index</t>
-  </si>
-  <si>
-    <t>AAPL-Q1-2013</t>
-  </si>
-  <si>
-    <t>AAPL-Q2-2013</t>
-  </si>
-  <si>
-    <t>AAPL-Q3-2013</t>
-  </si>
-  <si>
-    <t>AAPL-Q4-2013</t>
-  </si>
-  <si>
-    <t>AAPL-Q1-2014</t>
-  </si>
-  <si>
-    <t>AAPL-Q2-2014</t>
-  </si>
-  <si>
-    <t>AAPL-Q3-2014</t>
-  </si>
-  <si>
-    <t>AAPL-Q4-2014</t>
-  </si>
-  <si>
-    <t>AAPL-Q1-2015</t>
-  </si>
-  <si>
-    <t>AAPL-Q2-2015</t>
-  </si>
-  <si>
-    <t>AAPL-Q3-2015</t>
-  </si>
-  <si>
-    <t>AAPL-Q4-2015</t>
-  </si>
-  <si>
-    <t>AAPL-Q1-2016</t>
-  </si>
-  <si>
-    <t>AAPL-Q2-2016</t>
-  </si>
-  <si>
-    <t>AAPL-Q3-2016</t>
-  </si>
-  <si>
-    <t>AAPL-Q4-2016</t>
-  </si>
-  <si>
-    <t>AAPL-Q2-2017</t>
-  </si>
-  <si>
-    <t>AAPL-Q3-2017</t>
-  </si>
-  <si>
-    <t>AAPL-Q4-2017</t>
   </si>
   <si>
     <t>AAPL-Q1-2018</t>
@@ -500,7 +443,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -530,13 +473,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>16.6339282989502</v>
+        <v>48.54999923706055</v>
       </c>
       <c r="C3">
-        <v>13.75357055664062</v>
+        <v>40.15750122070312</v>
       </c>
       <c r="D3">
-        <v>15.3836774379015</v>
+        <v>45.34914070367813</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -544,13 +487,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>18.34785652160645</v>
+        <v>57.41749954223633</v>
       </c>
       <c r="C4">
-        <v>14.32928562164307</v>
+        <v>45.85499954223633</v>
       </c>
       <c r="D4">
-        <v>16.57310656895713</v>
+        <v>52.07500027853345</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -558,13 +501,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>20.54071426391602</v>
+        <v>58.36750030517578</v>
       </c>
       <c r="C5">
-        <v>16.94321441650391</v>
+        <v>36.64749908447266</v>
       </c>
       <c r="D5">
-        <v>18.82963716416132</v>
+        <v>48.6238710341915</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -572,13 +515,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>20.04571342468262</v>
+        <v>49.42250061035156</v>
       </c>
       <c r="C6">
-        <v>17.62678527832031</v>
+        <v>35.5</v>
       </c>
       <c r="D6">
-        <v>19.04820279152162</v>
+        <v>42.36786282447077</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -586,13 +529,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>23.76250076293945</v>
+        <v>53.82749938964844</v>
       </c>
       <c r="C7">
-        <v>18.26178550720215</v>
+        <v>42.56750106811523</v>
       </c>
       <c r="D7">
-        <v>21.2148867107573</v>
+        <v>48.72317468552362</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -600,13 +543,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>25.93499946594238</v>
+        <v>56.60499954223633</v>
       </c>
       <c r="C8">
-        <v>23.02249908447266</v>
+        <v>48.14500045776367</v>
       </c>
       <c r="D8">
-        <v>24.50210316975911</v>
+        <v>52.22126981947157</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -614,13 +557,13 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>29.9375</v>
+        <v>73.49250030517578</v>
       </c>
       <c r="C9">
-        <v>23.79500007629395</v>
+        <v>53.78250122070312</v>
       </c>
       <c r="D9">
-        <v>27.09765879313151</v>
+        <v>63.91999992491707</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -628,13 +571,13 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>33.40000152587891</v>
+        <v>81.96250152587891</v>
       </c>
       <c r="C10">
-        <v>26.15749931335449</v>
+        <v>53.15250015258789</v>
       </c>
       <c r="D10">
-        <v>30.05407253388436</v>
+        <v>73.84766111066264</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -642,13 +585,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>33.6349983215332</v>
+        <v>93.09500122070312</v>
       </c>
       <c r="C11">
-        <v>30.77499961853027</v>
+        <v>59.22499847412109</v>
       </c>
       <c r="D11">
-        <v>31.98785700116839</v>
+        <v>76.62730135236468</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -656,13 +599,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>33.24250030517578</v>
+        <v>137.9799957275391</v>
       </c>
       <c r="C12">
-        <v>23</v>
+        <v>87.81999969482422</v>
       </c>
       <c r="D12">
-        <v>29.46658730885339</v>
+        <v>108.2566264319041</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -670,13 +613,13 @@
         <v>15</v>
       </c>
       <c r="B13">
-        <v>30.95499992370605</v>
+        <v>134.4100036621094</v>
       </c>
       <c r="C13">
-        <v>26.39249992370605</v>
+        <v>107.3199996948242</v>
       </c>
       <c r="D13">
-        <v>28.64611107962472</v>
+        <v>119.12523808555</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -684,13 +627,13 @@
         <v>16</v>
       </c>
       <c r="B14">
-        <v>27.35750007629395</v>
+        <v>145.0899963378906</v>
       </c>
       <c r="C14">
-        <v>23.09749984741211</v>
+        <v>116.2099990844727</v>
       </c>
       <c r="D14">
-        <v>24.90032780756716</v>
+        <v>129.1027417336741</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -698,13 +641,13 @@
         <v>17</v>
       </c>
       <c r="B15">
-        <v>28.09749984741211</v>
+        <v>137.0700073242188</v>
       </c>
       <c r="C15">
-        <v>22.36750030517578</v>
+        <v>118.8600006103516</v>
       </c>
       <c r="D15">
-        <v>25.06824219226837</v>
+        <v>128.860476175944</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -712,13 +655,13 @@
         <v>18</v>
       </c>
       <c r="B16">
-        <v>29.04500007629395</v>
+        <v>157.2599945068359</v>
       </c>
       <c r="C16">
-        <v>22.875</v>
+        <v>133.3500061035156</v>
       </c>
       <c r="D16">
-        <v>26.13456353687105</v>
+        <v>146.9639684283544</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -726,13 +669,13 @@
         <v>19</v>
       </c>
       <c r="B17">
-        <v>29.67250061035156</v>
+        <v>182.1300048828125</v>
       </c>
       <c r="C17">
-        <v>26.02000045776367</v>
+        <v>138.2700042724609</v>
       </c>
       <c r="D17">
-        <v>28.34297791649314</v>
+        <v>155.4160320948041</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -740,13 +683,13 @@
         <v>20</v>
       </c>
       <c r="B18">
-        <v>36.125</v>
+        <v>182.9400024414062</v>
       </c>
       <c r="C18">
-        <v>28.69000053405762</v>
+        <v>150.1000061035156</v>
       </c>
       <c r="D18">
-        <v>32.92814507022981</v>
+        <v>168.4757145472935</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -754,320 +697,40 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>39.16249847412109</v>
+        <v>179.6100006103516</v>
       </c>
       <c r="C19">
-        <v>35.01499938964844</v>
+        <v>129.0399932861328</v>
       </c>
       <c r="D19">
-        <v>36.96884893992591</v>
+        <v>153.889032917638</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B20">
-        <v>41.23500061035156</v>
+        <v>176.1499938964844</v>
       </c>
       <c r="C20">
-        <v>35.60250091552734</v>
+        <v>133.7700042724609</v>
       </c>
       <c r="D20">
-        <v>38.7922620016431</v>
+        <v>156.6163489932106</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B21">
-        <v>44.29999923706055</v>
+        <v>157.5</v>
       </c>
       <c r="C21">
-        <v>38.1150016784668</v>
+        <v>125.870002746582</v>
       </c>
       <c r="D21">
-        <v>41.78706353808206</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22">
-        <v>45.875</v>
-      </c>
-      <c r="C22">
-        <v>37.56000137329102</v>
-      </c>
-      <c r="D22">
-        <v>43.04782792388416</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23">
-        <v>48.54999923706055</v>
-      </c>
-      <c r="C23">
-        <v>40.15750122070312</v>
-      </c>
-      <c r="D23">
-        <v>45.34914070367813</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24">
-        <v>57.41749954223633</v>
-      </c>
-      <c r="C24">
-        <v>45.85499954223633</v>
-      </c>
-      <c r="D24">
-        <v>52.07500027853345</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B25">
-        <v>58.36750030517578</v>
-      </c>
-      <c r="C25">
-        <v>36.64749908447266</v>
-      </c>
-      <c r="D25">
-        <v>48.6238710341915</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
-      <c r="A26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26">
-        <v>49.42250061035156</v>
-      </c>
-      <c r="C26">
-        <v>35.5</v>
-      </c>
-      <c r="D26">
-        <v>42.36786282447077</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B27">
-        <v>53.82749938964844</v>
-      </c>
-      <c r="C27">
-        <v>42.56750106811523</v>
-      </c>
-      <c r="D27">
-        <v>48.72317468552362</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>56.60499954223633</v>
-      </c>
-      <c r="C28">
-        <v>48.14500045776367</v>
-      </c>
-      <c r="D28">
-        <v>52.22126981947157</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29">
-        <v>73.49250030517578</v>
-      </c>
-      <c r="C29">
-        <v>53.78250122070312</v>
-      </c>
-      <c r="D29">
-        <v>63.91999992491707</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B30">
-        <v>81.96250152587891</v>
-      </c>
-      <c r="C30">
-        <v>53.15250015258789</v>
-      </c>
-      <c r="D30">
-        <v>73.84766111066264</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31">
-        <v>93.09500122070312</v>
-      </c>
-      <c r="C31">
-        <v>59.22499847412109</v>
-      </c>
-      <c r="D31">
-        <v>76.62730135236468</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B32">
-        <v>137.9799957275391</v>
-      </c>
-      <c r="C32">
-        <v>87.81999969482422</v>
-      </c>
-      <c r="D32">
-        <v>108.2566264319041</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B33">
-        <v>134.4100036621094</v>
-      </c>
-      <c r="C33">
-        <v>107.3199996948242</v>
-      </c>
-      <c r="D33">
-        <v>119.12523808555</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B34">
-        <v>145.0899963378906</v>
-      </c>
-      <c r="C34">
-        <v>116.2099990844727</v>
-      </c>
-      <c r="D34">
-        <v>129.1027417336741</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
-      <c r="A35" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B35">
-        <v>137.0700073242188</v>
-      </c>
-      <c r="C35">
-        <v>118.8600006103516</v>
-      </c>
-      <c r="D35">
-        <v>128.860476175944</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
-      <c r="A36" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B36">
-        <v>157.2599945068359</v>
-      </c>
-      <c r="C36">
-        <v>133.3500061035156</v>
-      </c>
-      <c r="D36">
-        <v>146.9639684283544</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
-      <c r="A37" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B37">
-        <v>182.1300048828125</v>
-      </c>
-      <c r="C37">
-        <v>138.2700042724609</v>
-      </c>
-      <c r="D37">
-        <v>155.4160320948041</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
-      <c r="A38" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B38">
-        <v>182.9400024414062</v>
-      </c>
-      <c r="C38">
-        <v>150.1000061035156</v>
-      </c>
-      <c r="D38">
-        <v>168.4757145472935</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
-      <c r="A39" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B39">
-        <v>179.6100006103516</v>
-      </c>
-      <c r="C39">
-        <v>129.0399932861328</v>
-      </c>
-      <c r="D39">
-        <v>153.889032917638</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="A40" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B40">
-        <v>176.1499938964844</v>
-      </c>
-      <c r="C40">
-        <v>133.7700042724609</v>
-      </c>
-      <c r="D40">
-        <v>156.6163489932106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
-      <c r="A41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B41">
-        <v>157.5</v>
-      </c>
-      <c r="C41">
-        <v>125.870002746582</v>
-      </c>
-      <c r="D41">
         <v>143.1830874050365</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added financial scores to the Company class
</commit_message>
<xml_diff>
--- a/Financial Modelling Prep Library/Company Financial Data/AAPL/quarter/stock_price_data.xlsx
+++ b/Financial Modelling Prep Library/Company Financial Data/AAPL/quarter/stock_price_data.xlsx
@@ -467,6 +467,15 @@
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B2">
+        <v>45.875</v>
+      </c>
+      <c r="C2">
+        <v>37.56000137329102</v>
+      </c>
+      <c r="D2">
+        <v>43.04782792388416</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="1" t="s">

</xml_diff>